<commit_message>
Add missing results for Konsta and Adam
</commit_message>
<xml_diff>
--- a/data/2020-08-25/SCW Weekly Comp 2020-08-25 (Responses).xlsx
+++ b/data/2020-08-25/SCW Weekly Comp 2020-08-25 (Responses).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-08-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA84A98C-7940-44C6-90B6-DE0009DA0283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14302667-E569-4F19-8A70-104196DD969B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="4740" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="344">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1034,6 +1034,27 @@
   </si>
   <si>
     <t>1:12.88</t>
+  </si>
+  <si>
+    <t>Adam Robson</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/599329904283159/?post_id=602657533950396&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>30 moves which I’m happy with. I have 23 to last 3 corner but only 1 cancellation 😭 made it in super quick time though so pretty happy.</t>
+  </si>
+  <si>
+    <t>Konsta Jukka</t>
+  </si>
+  <si>
+    <t>2008JUKK01</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/2812216602434889/?post_id=2812794762377073&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>Using 5 different cubes with different settings will be my this weeks excuse why my I was slower than my normal avg. 💩</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1064,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1060,6 +1081,18 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1075,7 +1108,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1083,11 +1116,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1095,8 +1144,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1313,11 +1378,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CY94"/>
+  <dimension ref="A1:DE96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96:DE96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4725,7 +4790,7 @@
         <v>17.16</v>
       </c>
     </row>
-    <row r="81" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>44074.810014305556</v>
       </c>
@@ -4766,7 +4831,7 @@
         <v>11.65</v>
       </c>
     </row>
-    <row r="82" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44074.810848692126</v>
       </c>
@@ -4807,7 +4872,7 @@
         <v>29.58</v>
       </c>
     </row>
-    <row r="83" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>44074.811942847227</v>
       </c>
@@ -4851,7 +4916,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="84" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44074.812923449077</v>
       </c>
@@ -4889,7 +4954,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44074.902765243052</v>
       </c>
@@ -4930,7 +4995,7 @@
         <v>35.32</v>
       </c>
     </row>
-    <row r="86" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44074.903411643521</v>
       </c>
@@ -4968,7 +5033,7 @@
         <v>46.82</v>
       </c>
     </row>
-    <row r="87" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44074.905134189816</v>
       </c>
@@ -5006,7 +5071,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="88" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44074.906653854167</v>
       </c>
@@ -5047,7 +5112,7 @@
         <v>14.38</v>
       </c>
     </row>
-    <row r="89" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44074.907780208334</v>
       </c>
@@ -5088,7 +5153,7 @@
         <v>27.19</v>
       </c>
     </row>
-    <row r="90" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44075.077119560185</v>
       </c>
@@ -5129,7 +5194,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="91" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44075.098254050929</v>
       </c>
@@ -5173,7 +5238,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="92" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44075.107897881942</v>
       </c>
@@ -5214,7 +5279,7 @@
         <v>25.63</v>
       </c>
     </row>
-    <row r="93" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:109" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44075.121313703705</v>
       </c>
@@ -5258,7 +5323,7 @@
         <v>24.33</v>
       </c>
     </row>
-    <row r="94" spans="1:93" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:109" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>44075.414695474537</v>
       </c>
@@ -5283,6 +5348,270 @@
       <c r="CJ94" s="3">
         <v>36</v>
       </c>
+    </row>
+    <row r="95" spans="1:109" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="7">
+        <v>43839.446805555555</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="8"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="8"/>
+      <c r="Q95" s="8"/>
+      <c r="R95" s="8"/>
+      <c r="S95" s="8"/>
+      <c r="T95" s="8"/>
+      <c r="U95" s="8"/>
+      <c r="V95" s="8"/>
+      <c r="W95" s="8"/>
+      <c r="X95" s="8"/>
+      <c r="Y95" s="8"/>
+      <c r="Z95" s="8"/>
+      <c r="AA95" s="8"/>
+      <c r="AB95" s="8"/>
+      <c r="AC95" s="8"/>
+      <c r="AD95" s="8"/>
+      <c r="AE95" s="8"/>
+      <c r="AF95" s="8"/>
+      <c r="AG95" s="8"/>
+      <c r="AH95" s="8"/>
+      <c r="AI95" s="8"/>
+      <c r="AJ95" s="8"/>
+      <c r="AK95" s="8"/>
+      <c r="AL95" s="8"/>
+      <c r="AM95" s="8"/>
+      <c r="AN95" s="8"/>
+      <c r="AO95" s="8"/>
+      <c r="AP95" s="8"/>
+      <c r="AQ95" s="8"/>
+      <c r="AR95" s="8"/>
+      <c r="AS95" s="8"/>
+      <c r="AT95" s="8"/>
+      <c r="AU95" s="8"/>
+      <c r="AV95" s="8"/>
+      <c r="AW95" s="8"/>
+      <c r="AX95" s="8"/>
+      <c r="AY95" s="8"/>
+      <c r="AZ95" s="8"/>
+      <c r="BA95" s="8"/>
+      <c r="BB95" s="8"/>
+      <c r="BC95" s="8"/>
+      <c r="BD95" s="8"/>
+      <c r="BE95" s="8"/>
+      <c r="BF95" s="8"/>
+      <c r="BG95" s="8"/>
+      <c r="BH95" s="8"/>
+      <c r="BI95" s="8"/>
+      <c r="BJ95" s="8"/>
+      <c r="BK95" s="8"/>
+      <c r="BL95" s="8"/>
+      <c r="BM95" s="8"/>
+      <c r="BN95" s="8"/>
+      <c r="BO95" s="8"/>
+      <c r="BP95" s="8"/>
+      <c r="BQ95" s="8"/>
+      <c r="BR95" s="8"/>
+      <c r="BS95" s="8"/>
+      <c r="BT95" s="8"/>
+      <c r="BU95" s="8"/>
+      <c r="BV95" s="8"/>
+      <c r="BW95" s="8"/>
+      <c r="BX95" s="8"/>
+      <c r="BY95" s="8"/>
+      <c r="BZ95" s="8"/>
+      <c r="CA95" s="8"/>
+      <c r="CB95" s="8"/>
+      <c r="CC95" s="8"/>
+      <c r="CD95" s="8"/>
+      <c r="CE95" s="8"/>
+      <c r="CF95" s="8"/>
+      <c r="CG95" s="8"/>
+      <c r="CH95" s="8"/>
+      <c r="CI95" s="8"/>
+      <c r="CJ95" s="11">
+        <v>30</v>
+      </c>
+      <c r="CK95" s="8"/>
+      <c r="CL95" s="8"/>
+      <c r="CM95" s="8"/>
+      <c r="CN95" s="8"/>
+      <c r="CO95" s="8"/>
+      <c r="CP95" s="8"/>
+      <c r="CQ95" s="8"/>
+      <c r="CR95" s="8"/>
+      <c r="CS95" s="8"/>
+      <c r="CT95" s="8"/>
+      <c r="CU95" s="8"/>
+      <c r="CV95" s="8"/>
+      <c r="CW95" s="8"/>
+      <c r="CX95" s="8"/>
+      <c r="CY95" s="8"/>
+      <c r="CZ95" s="8"/>
+      <c r="DA95" s="8"/>
+      <c r="DB95" s="8"/>
+      <c r="DC95" s="8"/>
+      <c r="DD95" s="8"/>
+      <c r="DE95" s="8"/>
+    </row>
+    <row r="96" spans="1:109" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="7">
+        <v>43839.452407407407</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+      <c r="N96" s="8"/>
+      <c r="O96" s="11">
+        <v>12.09</v>
+      </c>
+      <c r="P96" s="11">
+        <v>12.94</v>
+      </c>
+      <c r="Q96" s="11">
+        <v>13.8</v>
+      </c>
+      <c r="R96" s="11">
+        <v>11.27</v>
+      </c>
+      <c r="S96" s="11">
+        <v>14.52</v>
+      </c>
+      <c r="T96" s="11">
+        <v>11.27</v>
+      </c>
+      <c r="U96" s="11">
+        <v>12.94</v>
+      </c>
+      <c r="V96" s="8"/>
+      <c r="W96" s="8"/>
+      <c r="X96" s="8"/>
+      <c r="Y96" s="8"/>
+      <c r="Z96" s="8"/>
+      <c r="AA96" s="8"/>
+      <c r="AB96" s="8"/>
+      <c r="AC96" s="8"/>
+      <c r="AD96" s="8"/>
+      <c r="AE96" s="8"/>
+      <c r="AF96" s="8"/>
+      <c r="AG96" s="8"/>
+      <c r="AH96" s="8"/>
+      <c r="AI96" s="8"/>
+      <c r="AJ96" s="8"/>
+      <c r="AK96" s="8"/>
+      <c r="AL96" s="8"/>
+      <c r="AM96" s="8"/>
+      <c r="AN96" s="8"/>
+      <c r="AO96" s="8"/>
+      <c r="AP96" s="8"/>
+      <c r="AQ96" s="8"/>
+      <c r="AR96" s="8"/>
+      <c r="AS96" s="8"/>
+      <c r="AT96" s="8"/>
+      <c r="AU96" s="8"/>
+      <c r="AV96" s="8"/>
+      <c r="AW96" s="8"/>
+      <c r="AX96" s="8"/>
+      <c r="AY96" s="8"/>
+      <c r="AZ96" s="8"/>
+      <c r="BA96" s="8"/>
+      <c r="BB96" s="8"/>
+      <c r="BC96" s="8"/>
+      <c r="BD96" s="8"/>
+      <c r="BE96" s="8"/>
+      <c r="BF96" s="8"/>
+      <c r="BG96" s="8"/>
+      <c r="BH96" s="8"/>
+      <c r="BI96" s="8"/>
+      <c r="BJ96" s="8"/>
+      <c r="BK96" s="8"/>
+      <c r="BL96" s="8"/>
+      <c r="BM96" s="8"/>
+      <c r="BN96" s="8"/>
+      <c r="BO96" s="8"/>
+      <c r="BP96" s="8"/>
+      <c r="BQ96" s="8"/>
+      <c r="BR96" s="8"/>
+      <c r="BS96" s="8"/>
+      <c r="BT96" s="8"/>
+      <c r="BU96" s="8"/>
+      <c r="BV96" s="8"/>
+      <c r="BW96" s="8"/>
+      <c r="BX96" s="8"/>
+      <c r="BY96" s="8"/>
+      <c r="BZ96" s="8"/>
+      <c r="CA96" s="8"/>
+      <c r="CB96" s="8"/>
+      <c r="CC96" s="8"/>
+      <c r="CD96" s="8"/>
+      <c r="CE96" s="8"/>
+      <c r="CF96" s="8"/>
+      <c r="CG96" s="8"/>
+      <c r="CH96" s="8"/>
+      <c r="CI96" s="8"/>
+      <c r="CJ96" s="8"/>
+      <c r="CK96" s="8"/>
+      <c r="CL96" s="8"/>
+      <c r="CM96" s="8"/>
+      <c r="CN96" s="8"/>
+      <c r="CO96" s="8"/>
+      <c r="CP96" s="8"/>
+      <c r="CQ96" s="8"/>
+      <c r="CR96" s="8"/>
+      <c r="CS96" s="8"/>
+      <c r="CT96" s="8"/>
+      <c r="CU96" s="8"/>
+      <c r="CV96" s="8"/>
+      <c r="CW96" s="8"/>
+      <c r="CX96" s="8"/>
+      <c r="CY96" s="8"/>
+      <c r="CZ96" s="8"/>
+      <c r="DA96" s="8"/>
+      <c r="DB96" s="8"/>
+      <c r="DC96" s="8"/>
+      <c r="DD96" s="8"/>
+      <c r="DE96" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:CY94" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -5380,7 +5709,10 @@
     <hyperlink ref="F92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
     <hyperlink ref="F93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="F94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="F95" r:id="rId94" xr:uid="{5047D243-C972-43E4-842E-E99F9EE2EA6B}"/>
+    <hyperlink ref="F96" r:id="rId95" xr:uid="{9B935824-B4CA-4E02-927A-D3F5D27E5D04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId96"/>
 </worksheet>
 </file>
</xml_diff>